<commit_message>
Cleaned code to highlight animals outucome
</commit_message>
<xml_diff>
--- a/Project3/Reports/Table1Demographics_formatted.xlsx
+++ b/Project3/Reports/Table1Demographics_formatted.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Overall</t>
   </si>
@@ -33,103 +33,127 @@
     <t>n</t>
   </si>
   <si>
+    <t>17.49 (7.48)</t>
+  </si>
+  <si>
+    <t>16.42 (8.22)</t>
+  </si>
+  <si>
+    <t>19.35 (5.54)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8.82 (4.05)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8.23 (4.41)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9.87 (3.08)</t>
+  </si>
+  <si>
     <t>Male</t>
   </si>
   <si>
-    <t xml:space="preserve">   91 (42.1) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   67 (46.2) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   24 (33.8) </t>
+    <t xml:space="preserve">   82 (43.9) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   59 (49.6) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   23 (33.8) </t>
   </si>
   <si>
     <t>Female</t>
   </si>
   <si>
-    <t xml:space="preserve">  125 (57.9) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   78 (53.8) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   47 (66.2) </t>
+    <t xml:space="preserve">  105 (56.1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   60 (50.4) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   45 (66.2) </t>
   </si>
   <si>
     <t>SES (mean (sd))</t>
   </si>
   <si>
-    <t>49.10 (11.54)</t>
-  </si>
-  <si>
-    <t>49.15 (10.86)</t>
-  </si>
-  <si>
-    <t>49.01 (12.89)</t>
-  </si>
-  <si>
-    <t>80.05 (9.22)</t>
-  </si>
-  <si>
-    <t>77.72 (9.62)</t>
-  </si>
-  <si>
-    <t>84.80 (6.07)</t>
-  </si>
-  <si>
-    <t>24.56 (9.30)</t>
-  </si>
-  <si>
-    <t>25.83 (9.36)</t>
-  </si>
-  <si>
-    <t>21.99 (8.68)</t>
-  </si>
-  <si>
-    <t>18.11 (4.94)</t>
-  </si>
-  <si>
-    <t>18.73 (4.93)</t>
-  </si>
-  <si>
-    <t>16.53 (4.63)</t>
-  </si>
-  <si>
-    <t>13.63 (4.32)</t>
-  </si>
-  <si>
-    <t>14.40 (4.09)</t>
-  </si>
-  <si>
-    <t>12.07 (4.39)</t>
-  </si>
-  <si>
-    <t>11.20 (4.86)</t>
-  </si>
-  <si>
-    <t>12.28 (4.55)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 9.01 (4.75)</t>
+    <t>49.32 (11.68)</t>
+  </si>
+  <si>
+    <t>49.66 (10.86)</t>
+  </si>
+  <si>
+    <t>48.74 (13.07)</t>
+  </si>
+  <si>
+    <t>80.10 (8.87)</t>
+  </si>
+  <si>
+    <t>77.16 (8.92)</t>
+  </si>
+  <si>
+    <t>85.24 (6.01)</t>
+  </si>
+  <si>
+    <t>24.56 (9.36)</t>
+  </si>
+  <si>
+    <t>26.52 (9.43)</t>
+  </si>
+  <si>
+    <t>21.12 (8.22)</t>
+  </si>
+  <si>
+    <t>17.33 (5.11)</t>
+  </si>
+  <si>
+    <t>18.30 (4.99)</t>
+  </si>
+  <si>
+    <t>15.62 (4.91)</t>
+  </si>
+  <si>
+    <t>13.48 (4.36)</t>
+  </si>
+  <si>
+    <t>14.60 (4.02)</t>
+  </si>
+  <si>
+    <t>11.53 (4.28)</t>
+  </si>
+  <si>
+    <t>11.13 (5.00)</t>
+  </si>
+  <si>
+    <t>12.55 (4.51)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8.65 (4.88)</t>
+  </si>
+  <si>
+    <t>Number observations (mean (sd))</t>
+  </si>
+  <si>
+    <t>Years of follow-up (mean (sd))</t>
+  </si>
+  <si>
+    <t>Gender (%)</t>
   </si>
   <si>
     <t>Age (mean (sd))</t>
   </si>
   <si>
-    <t>Category fluency for animals score (mean (sd))</t>
-  </si>
-  <si>
-    <t>Logical memory I Story A score (mean (sd))</t>
-  </si>
-  <si>
-    <t>Logical memory II Story A score (mean (sd))</t>
-  </si>
-  <si>
-    <t>Block design test score (mean (sd))</t>
-  </si>
-  <si>
-    <t>Gender (n (%))</t>
+    <t>BlockR (mean (sd))</t>
+  </si>
+  <si>
+    <t>Animals (mean (sd))</t>
+  </si>
+  <si>
+    <t>LogMemI (mean (sd))</t>
+  </si>
+  <si>
+    <t>LogMemII (mean (sd))</t>
   </si>
 </sst>
 </file>
@@ -466,7 +490,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -601,6 +625,30 @@
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -655,43 +703,33 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1013,180 +1051,191 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" style="13" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="32.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="9"/>
+    <col min="3" max="3" width="12.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="15"/>
+      <c r="B1" s="8"/>
       <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="16"/>
       <c r="C2" s="12">
-        <v>216</v>
-      </c>
-      <c r="D2" s="12">
-        <v>145</v>
-      </c>
-      <c r="E2" s="8">
-        <v>71</v>
-      </c>
-      <c r="F2" s="7"/>
+        <v>187</v>
+      </c>
+      <c r="D2" s="1">
+        <v>119</v>
+      </c>
+      <c r="E2" s="1">
+        <v>68</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="17" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>7</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="12" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="C5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="12" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="C6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="8" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" s="9" customFormat="1" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="16"/>
       <c r="C7" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" s="9" customFormat="1" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="16"/>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="C8" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" s="9" customFormat="1" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="16"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="C9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" s="9" customFormat="1" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="16"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="C10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>